<commit_message>
notizen für excel berechnung
</commit_message>
<xml_diff>
--- a/src/main/resources/Beispiel-Niklas.xlsx
+++ b/src/main/resources/Beispiel-Niklas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jana2/Documents/LfS/Betreuung/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Blumenroth\ideaProjects\Masterarbeit\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A122F4B6-89E9-C74F-A37C-18197AAB09D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{043C181D-3984-42A6-8D3B-A6443074B62E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21900" xr2:uid="{947A9DF4-7017-6D48-893C-1CEE0C78246B}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{947A9DF4-7017-6D48-893C-1CEE0C78246B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,17 +24,6 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
@@ -42,7 +31,7 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
   <connection id="1" xr16:uid="{B95AF660-98BE-8142-AB3B-E04DB3439E6C}" name="52-CMAA-Report" type="6" refreshedVersion="8" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/jana2/Documents/Digital Facilitator 2/output_files/2023-5-31-11:52-CMAA-Report.csv" decimal="," thousands="." semicolon="1">
+    <textPr sourceFile="/Users/jana2/Documents/Digital Facilitator 2/output_files/2023-5-31-11:52-CMAA-Report.csv" decimal="," thousands="." semicolon="1">
       <textFields count="5">
         <textField/>
         <textField/>
@@ -56,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="68">
   <si>
     <t xml:space="preserve">Resolution Recommendation: </t>
   </si>
@@ -269,12 +258,42 @@
   <si>
     <t>Instanzen</t>
   </si>
+  <si>
+    <t>Wie oft hat eine Alternative welchen Rang erreicht hat?</t>
+  </si>
+  <si>
+    <t>Welche Entropie kann ich mit einer bestimmten Auflösung erreichen?</t>
+  </si>
+  <si>
+    <t>Für Rang 1: In wie vielen Fällen hat A1 gewonnen für ein bestimmtes Judgement?</t>
+  </si>
+  <si>
+    <t>Nach Formel</t>
+  </si>
+  <si>
+    <t>Alle Konflikte ergeben 0,49...</t>
+  </si>
+  <si>
+    <t>Alle Konflikte ergeben 0,33...</t>
+  </si>
+  <si>
+    <t>Alle Konflikte ergeben 0,17...</t>
+  </si>
+  <si>
+    <t>Siehe Current Judgement..</t>
+  </si>
+  <si>
+    <t>Nach Formel + normalisiert</t>
+  </si>
+  <si>
+    <t>Rang 1 Werte normailieren und Formel nutzen</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -416,7 +435,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -448,12 +467,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -469,12 +482,12 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -587,7 +600,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -883,34 +896,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E55D6BED-C0C5-2D4D-AB92-5D2A25E0FAB2}">
-  <dimension ref="A1:K109"/>
+  <dimension ref="A1:Q109"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="185" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" zoomScale="89" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="15.5"/>
   <cols>
     <col min="1" max="1" width="8.33203125" style="2"/>
     <col min="2" max="16384" width="8.33203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11">
       <c r="A1" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11">
       <c r="A3" s="7" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D3" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
       <c r="A5" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11">
       <c r="A7" s="2" t="s">
         <v>1</v>
       </c>
@@ -927,7 +943,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11">
       <c r="A8" s="2">
         <v>1.0552699999999999</v>
       </c>
@@ -944,7 +960,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11">
       <c r="A10" s="7" t="s">
         <v>7</v>
       </c>
@@ -952,7 +968,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11">
       <c r="A12" s="3"/>
       <c r="B12" s="5" t="s">
         <v>8</v>
@@ -985,7 +1001,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11">
       <c r="A13" s="3" t="s">
         <v>12</v>
       </c>
@@ -1020,7 +1036,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11">
       <c r="A14" s="3" t="s">
         <v>13</v>
       </c>
@@ -1055,7 +1071,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11">
       <c r="A15" s="3" t="s">
         <v>14</v>
       </c>
@@ -1090,12 +1106,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12">
       <c r="A18" s="7" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12">
       <c r="A20" s="5" t="s">
         <v>12</v>
       </c>
@@ -1127,7 +1143,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12">
       <c r="A21" s="10" t="s">
         <v>41</v>
       </c>
@@ -1159,12 +1175,15 @@
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:12">
       <c r="A24" s="7" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E24" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12">
       <c r="A26" s="3"/>
       <c r="B26" s="4" t="s">
         <v>19</v>
@@ -1179,7 +1198,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:12">
       <c r="A27" s="3" t="s">
         <v>22</v>
       </c>
@@ -1196,7 +1215,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:12">
       <c r="A28" s="3" t="s">
         <v>23</v>
       </c>
@@ -1213,7 +1232,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:12">
       <c r="A29" s="3" t="s">
         <v>24</v>
       </c>
@@ -1230,12 +1249,18 @@
         <v>9</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:12">
       <c r="A32" s="7" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="E32" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="L32" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11">
       <c r="A34" s="3"/>
       <c r="B34" s="5" t="s">
         <v>8</v>
@@ -1268,7 +1293,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:11">
       <c r="A35" s="3" t="s">
         <v>12</v>
       </c>
@@ -1303,7 +1328,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:11">
       <c r="A36" s="3" t="s">
         <v>13</v>
       </c>
@@ -1338,7 +1363,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:11">
       <c r="A37" s="3" t="s">
         <v>14</v>
       </c>
@@ -1373,12 +1398,15 @@
         <v>9</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:11">
       <c r="A40" s="7" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D40" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11">
       <c r="A42" s="5" t="s">
         <v>12</v>
       </c>
@@ -1410,7 +1438,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:11">
       <c r="A43" s="3">
         <v>1.39693</v>
       </c>
@@ -1442,17 +1470,23 @@
         <v>9</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:11">
       <c r="A46" s="7" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F46" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11">
       <c r="A47" s="2" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C47" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="49" spans="1:17">
       <c r="B49" s="1" t="s">
         <v>8</v>
       </c>
@@ -1484,7 +1518,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:17">
       <c r="A50" s="2" t="s">
         <v>12</v>
       </c>
@@ -1518,8 +1552,11 @@
       <c r="K50" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="N50" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="51" spans="1:17">
       <c r="A51" s="2" t="s">
         <v>13</v>
       </c>
@@ -1553,8 +1590,9 @@
       <c r="K51" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="N51" s="2"/>
+    </row>
+    <row r="52" spans="1:17">
       <c r="A52" s="2" t="s">
         <v>14</v>
       </c>
@@ -1588,13 +1626,66 @@
       <c r="K52" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="N52" s="3"/>
+      <c r="O52" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P52" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q52" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="53" spans="1:17">
+      <c r="N53" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="O53" s="4">
+        <v>0.33912037037037002</v>
+      </c>
+      <c r="P53" s="4">
+        <v>0.436921296296296</v>
+      </c>
+      <c r="Q53" s="4">
+        <v>0.22395833333333301</v>
+      </c>
+    </row>
+    <row r="54" spans="1:17">
+      <c r="N54" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="O54" s="4">
+        <v>0.49645543981481399</v>
+      </c>
+      <c r="P54" s="4">
+        <v>0.35923032407407401</v>
+      </c>
+      <c r="Q54" s="4">
+        <v>0.14431423611111099</v>
+      </c>
+    </row>
+    <row r="55" spans="1:17">
       <c r="A55" s="2" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C55" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="N55" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="O55" s="4">
+        <v>0.17599826388888801</v>
+      </c>
+      <c r="P55" s="4">
+        <v>0.20240162037036999</v>
+      </c>
+      <c r="Q55" s="4">
+        <v>0.62160011574074003</v>
+      </c>
+    </row>
+    <row r="57" spans="1:17">
       <c r="B57" s="1" t="s">
         <v>8</v>
       </c>
@@ -1626,7 +1717,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:17">
       <c r="A58" s="2" t="s">
         <v>12</v>
       </c>
@@ -1661,7 +1752,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:17">
       <c r="A59" s="2" t="s">
         <v>13</v>
       </c>
@@ -1696,7 +1787,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:17">
       <c r="A60" s="2" t="s">
         <v>14</v>
       </c>
@@ -1731,12 +1822,15 @@
         <v>9</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:17">
       <c r="A63" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C63" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11">
       <c r="B65" s="1" t="s">
         <v>8</v>
       </c>
@@ -1768,7 +1862,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:11">
       <c r="A66" s="2" t="s">
         <v>12</v>
       </c>
@@ -1803,7 +1897,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:11">
       <c r="A67" s="2" t="s">
         <v>13</v>
       </c>
@@ -1838,7 +1932,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:11">
       <c r="A68" s="2" t="s">
         <v>14</v>
       </c>
@@ -1873,17 +1967,17 @@
         <v>9</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:11">
       <c r="A71" s="7" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:11">
       <c r="A72" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:11">
       <c r="B74" s="1" t="s">
         <v>8</v>
       </c>
@@ -1915,7 +2009,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:11">
       <c r="A75" s="2" t="s">
         <v>12</v>
       </c>
@@ -1950,7 +2044,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:11">
       <c r="A76" s="2" t="s">
         <v>13</v>
       </c>
@@ -1985,7 +2079,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:11">
       <c r="A77" s="2" t="s">
         <v>14</v>
       </c>
@@ -2020,12 +2114,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:11">
       <c r="A80" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:11">
       <c r="B82" s="1" t="s">
         <v>8</v>
       </c>
@@ -2057,7 +2151,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:11">
       <c r="A83" s="2" t="s">
         <v>12</v>
       </c>
@@ -2092,7 +2186,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:11">
       <c r="A84" s="2" t="s">
         <v>13</v>
       </c>
@@ -2127,7 +2221,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:11">
       <c r="A85" s="2" t="s">
         <v>14</v>
       </c>
@@ -2162,12 +2256,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:11">
       <c r="A88" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:11">
       <c r="B90" s="1" t="s">
         <v>8</v>
       </c>
@@ -2199,7 +2293,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:11">
       <c r="A91" s="2" t="s">
         <v>12</v>
       </c>
@@ -2234,7 +2328,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:11">
       <c r="A92" s="2" t="s">
         <v>13</v>
       </c>
@@ -2269,7 +2363,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:11">
       <c r="A93" s="2" t="s">
         <v>14</v>
       </c>
@@ -2304,12 +2398,15 @@
         <v>9</v>
       </c>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:11">
       <c r="A96" s="7" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="G96" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="98" spans="1:11">
       <c r="B98" s="1" t="s">
         <v>12</v>
       </c>
@@ -2329,7 +2426,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:11">
       <c r="A99" s="2" t="s">
         <v>22</v>
       </c>
@@ -2364,7 +2461,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:11">
       <c r="A100" s="2" t="s">
         <v>23</v>
       </c>
@@ -2399,7 +2496,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:11">
       <c r="A101" s="2" t="s">
         <v>24</v>
       </c>
@@ -2434,12 +2531,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:11">
       <c r="A104" s="7" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:11">
       <c r="B106" s="1" t="s">
         <v>12</v>
       </c>
@@ -2459,7 +2556,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:11">
       <c r="A107" s="2" t="s">
         <v>22</v>
       </c>
@@ -2494,7 +2591,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:11">
       <c r="A108" s="2" t="s">
         <v>23</v>
       </c>
@@ -2529,7 +2626,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:11">
       <c r="A109" s="2" t="s">
         <v>24</v>
       </c>
@@ -2590,9 +2687,9 @@
       <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10">
       <c r="A1" s="3"/>
       <c r="B1" s="5" t="s">
         <v>8</v>
@@ -2622,7 +2719,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10">
       <c r="A2" s="3" t="s">
         <v>12</v>
       </c>
@@ -2654,7 +2751,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10">
       <c r="A3" s="3" t="s">
         <v>13</v>
       </c>
@@ -2686,7 +2783,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10">
       <c r="A4" s="3" t="s">
         <v>14</v>
       </c>
@@ -2718,12 +2815,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A7" s="11" t="s">
+    <row r="7" spans="1:10">
+      <c r="A7" s="2" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10">
       <c r="A9" s="3"/>
       <c r="B9" s="5" t="s">
         <v>8</v>
@@ -2735,49 +2832,49 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10">
       <c r="A10" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="12" t="s">
+      <c r="B10" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="C10" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="D10" s="12" t="s">
+      <c r="D10" s="4" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10">
       <c r="A11" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="12" t="s">
+      <c r="B11" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C11" s="12" t="s">
+      <c r="C11" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="D11" s="12" t="s">
+      <c r="D11" s="4" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10">
       <c r="A12" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="12" t="s">
+      <c r="B12" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="C12" s="12" t="s">
+      <c r="C12" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="D12" s="12" t="s">
+      <c r="D12" s="4" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10">
       <c r="A14" s="3"/>
       <c r="B14" s="5" t="s">
         <v>8</v>
@@ -2789,104 +2886,104 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10">
       <c r="A15" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="12" t="s">
+      <c r="B15" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="C15" s="12" t="s">
+      <c r="C15" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="D15" s="12" t="s">
+      <c r="D15" s="4" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10">
       <c r="A16" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="12" t="s">
+      <c r="B16" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C16" s="12" t="s">
+      <c r="C16" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="D16" s="12" t="s">
+      <c r="D16" s="4" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4">
       <c r="A17" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B17" s="12" t="s">
+      <c r="B17" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="C17" s="12" t="s">
+      <c r="C17" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="D17" s="12" t="s">
+      <c r="D17" s="4" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="13"/>
-      <c r="B19" s="14" t="s">
+    <row r="19" spans="1:4">
+      <c r="A19" s="11"/>
+      <c r="B19" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="C19" s="14" t="s">
+      <c r="C19" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="D19" s="15" t="s">
+      <c r="D19" s="13" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="16" t="s">
+    <row r="20" spans="1:4">
+      <c r="A20" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B20" s="17" t="s">
+      <c r="B20" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="C20" s="17" t="s">
+      <c r="C20" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="D20" s="17" t="s">
+      <c r="D20" s="15" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="16" t="s">
+    <row r="21" spans="1:4">
+      <c r="A21" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="B21" s="17" t="s">
+      <c r="B21" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="C21" s="17" t="s">
+      <c r="C21" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="D21" s="17" t="s">
+      <c r="D21" s="15" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="16" t="s">
+    <row r="22" spans="1:4">
+      <c r="A22" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="B22" s="17" t="s">
+      <c r="B22" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="C22" s="17" t="s">
+      <c r="C22" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="D22" s="17" t="s">
+      <c r="D22" s="15" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" s="18" t="s">
+    <row r="24" spans="1:4">
+      <c r="A24" s="16" t="s">
         <v>56</v>
       </c>
     </row>

</xml_diff>